<commit_message>
Implement parser of Table definition sheets.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoKeyGeneratorKtBucketStructure.xlsx
+++ b/meta/program/BlancoKeyGeneratorKtBucketStructure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoKeyGeneratorKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC578AD3-5E90-B245-9001-251F8BEF9A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EB8764-A978-7A47-987F-8452B6257477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10260" yWindow="6340" windowWidth="28300" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -298,6 +298,37 @@
     <t>bucket構成のバージョンです。</t>
     <rPh sb="6" eb="8">
       <t xml:space="preserve">コウセイ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>tableMap</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>new java.util.HashMap&lt;java.lang.String, blanco.keygeneratorkt.valueobject.BlancoKeyGeneratorKtTableStructure&gt;()</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>java.util.Map&lt;java.lang.String, blanco.keygeneratorkt.valueobject.BlancoKeyGeneratorKtTableStructure&gt;</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>このバケットに配置するテーブルです。table番号をキーにMapに保管することで、テーブル番号の重複を防ぎます。</t>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">ハイチスル </t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t xml:space="preserve">バンゴウ </t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t xml:space="preserve">ホカｎ </t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t xml:space="preserve">ジュウフク </t>
+    </rPh>
+    <rPh sb="51" eb="52">
+      <t xml:space="preserve">フセギマス。 </t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -1261,7 +1292,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1578,7 +1609,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="40">
-        <f t="shared" ref="A29:A33" si="0">A28+1</f>
+        <f t="shared" ref="A29:A34" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="41" t="s">
@@ -1668,13 +1699,24 @@
       <c r="F33" s="49"/>
       <c r="G33"/>
     </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="40"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="43"/>
+    <row r="34" spans="1:7" ht="105">
+      <c r="A34" s="40">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="56"/>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7">
@@ -1840,7 +1882,7 @@
       <c r="G54"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
     <mergeCell ref="E43:F43"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="E25:E26"/>
@@ -1854,6 +1896,7 @@
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">

</xml_diff>